<commit_message>
add some external modules/components
</commit_message>
<xml_diff>
--- a/Production/Components_And_Links.xlsx
+++ b/Production/Components_And_Links.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="19155" windowHeight="7500"/>
+    <workbookView xWindow="2760" yWindow="6030" windowWidth="19635" windowHeight="6300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,9 +165,6 @@
     <t>MSS22D18DIP</t>
   </si>
   <si>
-    <t>RESET</t>
-  </si>
-  <si>
     <t>Switch-PB-6.2x6.2-2-PIN-DIP</t>
   </si>
   <si>
@@ -313,13 +310,16 @@
   </si>
   <si>
     <t>DIODE</t>
+  </si>
+  <si>
+    <t>BUTTON</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,6 +340,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -402,11 +415,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -711,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,445 +754,445 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="F3" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E4" s="3">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3">
+        <v>4</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="3">
         <v>5</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="F9" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="3">
+        <v>2</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E15" s="3">
         <v>4</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="4">
-        <v>2</v>
-      </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="F15" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="3">
         <v>4</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="F19" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="4">
+      <c r="B21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="3">
         <v>5</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4">
-        <v>1</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="4">
-        <v>2</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="4">
-        <v>1</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="4">
-        <v>4</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="4">
-        <v>1</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="4">
-        <v>1</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="4">
-        <v>1</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="4">
-        <v>4</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="4">
-        <v>1</v>
-      </c>
-      <c r="F20" s="5" t="s">
+      <c r="F21" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="3" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="4">
-        <v>5</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="3" t="s">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="4">
-        <v>1</v>
-      </c>
-      <c r="F22" s="5" t="s">
+      <c r="B23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" s="4">
-        <v>1</v>
-      </c>
-      <c r="F23" s="5" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="5" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="4" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>